<commit_message>
Finished initial normalization + updated data_dictionary
</commit_message>
<xml_diff>
--- a/docs/Metadata/data_dictionary.xlsx
+++ b/docs/Metadata/data_dictionary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calin\Downloads\Project_DataTools\DT_Project\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calin\Downloads\Project_DataTools\DT_Project\docs\Metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DC1F69E-A028-42AF-973B-F1321A4BE000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA494263-2539-48AE-8D27-411C7F897B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{89D4B400-3AC8-43AB-AD49-7A475CCFE9AC}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="33">
   <si>
     <t>Column</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t># -  acts as placeholder for any digit</t>
+  </si>
+  <si>
+    <t>Gets defaulted to review</t>
+  </si>
+  <si>
+    <t>system_a, system_b, system_c, manual_entry, import_batch</t>
+  </si>
+  <si>
+    <t>Gets defaulted to import_batch</t>
   </si>
 </sst>
 </file>
@@ -501,7 +510,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -593,7 +602,7 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -624,10 +633,10 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -644,7 +653,7 @@
         <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Finished workflow + small changes to scripts
</commit_message>
<xml_diff>
--- a/docs/Metadata/data_dictionary.xlsx
+++ b/docs/Metadata/data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calin\Downloads\Project_DataTools\DT_Project\docs\Metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA494263-2539-48AE-8D27-411C7F897B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9640AC72-12A4-4F8C-8BFB-861BD10FC05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{89D4B400-3AC8-43AB-AD49-7A475CCFE9AC}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="36">
   <si>
     <t>Column</t>
   </si>
@@ -129,13 +129,22 @@
     <t># -  acts as placeholder for any digit</t>
   </si>
   <si>
-    <t>Gets defaulted to review</t>
-  </si>
-  <si>
     <t>system_a, system_b, system_c, manual_entry, import_batch</t>
   </si>
   <si>
-    <t>Gets defaulted to import_batch</t>
+    <t>placeholder: high</t>
+  </si>
+  <si>
+    <t>placeholder:ADMIN</t>
+  </si>
+  <si>
+    <t>placeholder:review</t>
+  </si>
+  <si>
+    <t>placeholder:import_batch</t>
+  </si>
+  <si>
+    <t>placeholder:CHK</t>
   </si>
 </sst>
 </file>
@@ -510,7 +519,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -619,7 +628,7 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -633,10 +642,10 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -653,7 +662,7 @@
         <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -671,7 +680,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F8" sqref="E2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -758,7 +767,7 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -775,7 +784,7 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -792,7 +801,7 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -809,7 +818,7 @@
         <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -826,7 +835,7 @@
         <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -843,7 +852,7 @@
         <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>